<commit_message>
Adjustment to pickup size and fps view for each items + put in item for puzzle + addressable group
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/Localization/EN/LocalizationEN_Item.xlsx
+++ b/Assets/Data/Excel/Localization/EN/LocalizationEN_Item.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\Localization\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9BC338-D345-4A50-B07A-5254B0DFD31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB6BF4C-3024-480D-9F3B-BDB4331CDC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
@@ -48,12 +48,6 @@
     <t>Item_2</t>
   </si>
   <si>
-    <t>Item_3</t>
-  </si>
-  <si>
-    <t>Item_4</t>
-  </si>
-  <si>
     <t>itemType</t>
   </si>
   <si>
@@ -63,10 +57,16 @@
     <t>This is Item 2</t>
   </si>
   <si>
-    <t>This is Item 3</t>
-  </si>
-  <si>
-    <t>This is Item 4</t>
+    <t>Item_PuzzleBlock_A</t>
+  </si>
+  <si>
+    <t>Item_PuzzleBlock_B</t>
+  </si>
+  <si>
+    <t>itemType is an enum</t>
+  </si>
+  <si>
+    <t>A puzzle block. Seems to be a part of some puzzle.</t>
   </si>
 </sst>
 </file>
@@ -451,14 +451,14 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.88671875" customWidth="1"/>
     <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -468,7 +468,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -483,7 +483,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -494,7 +497,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -502,10 +505,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -513,7 +516,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Locked door with key to open
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/Localization/EN/LocalizationEN_Item.xlsx
+++ b/Assets/Data/Excel/Localization/EN/LocalizationEN_Item.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\Localization\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB6BF4C-3024-480D-9F3B-BDB4331CDC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4797BE4E-F8CA-4AB2-93C3-746595775B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>A puzzle block. Seems to be a part of some puzzle.</t>
+  </si>
+  <si>
+    <t>Item_Key_A</t>
+  </si>
+  <si>
+    <t>A key to a door.</t>
   </si>
 </sst>
 </file>
@@ -448,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,6 +528,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>